<commit_message>
Message & file changes
</commit_message>
<xml_diff>
--- a/Whatsapp List_Main.xlsx
+++ b/Whatsapp List_Main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braya\Desktop\0. Whatsapp Web Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85C3995-8727-427B-8CF6-ED8747666F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8521C754-CE83-40B4-9C82-09EDFA0DDB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>S.no</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>529601172528</t>
+  </si>
+  <si>
+    <t>ING Gabriela</t>
+  </si>
+  <si>
+    <t>529611701291</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,6 +126,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,6 +446,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>